<commit_message>
Add api to create fields dynamic in xlsx form
</commit_message>
<xml_diff>
--- a/src/modules/field-management/router/exports/export_64f0329fd3041fb839d86be8.xlsx
+++ b/src/modules/field-management/router/exports/export_64f0329fd3041fb839d86be8.xlsx
@@ -4,10 +4,33 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Asset Identification Grp-Field2</t>
+  </si>
+  <si>
+    <t>Asset Identification Grp-Field1</t>
+  </si>
+  <si>
+    <t>Asset Identification Sub-Field1</t>
+  </si>
+  <si>
+    <t>Asset Identification Sub-Field2</t>
+  </si>
+  <si>
+    <t>Asset Identification Sub-Field3</t>
+  </si>
+  <si>
+    <t>Asset Identification Sub-Field4</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,9 +405,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="6" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>